<commit_message>
added comment and error fields
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmurphy/wit/archive/2025-26/modules/Discrete_Mathematics/exams/study_dashboard/Discrete_Mathematics_Exam_Viewer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0479B04B-EC1A-F747-94F8-B417236D3B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58347C62-2D6A-AD4D-AF30-4BA4641B8487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="11320" xr2:uid="{422AB7C4-DC60-EF4B-B76F-C5BB3A29986B}"/>
+    <workbookView xWindow="0" yWindow="2640" windowWidth="30240" windowHeight="15100" xr2:uid="{422AB7C4-DC60-EF4B-B76F-C5BB3A29986B}"/>
   </bookViews>
   <sheets>
     <sheet name="questions_2" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="151">
   <si>
     <t>paper</t>
   </si>
@@ -461,6 +461,18 @@
   </si>
   <si>
     <t>Verify logical propositions are logically equivalent.  Construct a truth table. Classify a logical proposition.</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>Error in solution - solution given is from an earlier version of this question.</t>
+  </si>
+  <si>
+    <t>Error in solution - the calculation of path through (5,3) is incorrect.</t>
+  </si>
+  <si>
+    <t>Error in solution - the calculation shown for (iii) is from an earlier version of the question.</t>
   </si>
 </sst>
 </file>
@@ -1321,11 +1333,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C95249E-C714-E54A-906E-011FA13AE7C6}">
-  <dimension ref="A1:L82"/>
+  <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="214" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="214" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1340,7 +1352,7 @@
     <col min="9" max="10" width="5.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1377,8 +1389,11 @@
       <c r="L1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1410,7 +1425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1442,7 +1457,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1474,7 +1489,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1506,7 +1521,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1538,7 +1553,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -1569,8 +1584,11 @@
       <c r="J7">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1602,7 +1620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -1634,7 +1652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1666,7 +1684,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -1698,7 +1716,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -1730,7 +1748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -1762,7 +1780,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -1794,7 +1812,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -1826,7 +1844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -1858,7 +1876,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -1893,7 +1911,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1925,7 +1943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -1957,7 +1975,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -1992,7 +2010,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -2024,7 +2042,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -2056,7 +2074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -2088,7 +2106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>75</v>
       </c>
@@ -2120,7 +2138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>75</v>
       </c>
@@ -2152,7 +2170,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -2184,7 +2202,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>75</v>
       </c>
@@ -2216,7 +2234,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>75</v>
       </c>
@@ -2248,7 +2266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>75</v>
       </c>
@@ -2280,7 +2298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -2312,7 +2330,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>75</v>
       </c>
@@ -2343,8 +2361,11 @@
       <c r="J31">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M31" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -2376,7 +2397,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>75</v>
       </c>
@@ -2408,7 +2429,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -2440,7 +2461,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>99</v>
       </c>
@@ -2472,7 +2493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>99</v>
       </c>
@@ -2504,7 +2525,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>99</v>
       </c>
@@ -2539,7 +2560,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>99</v>
       </c>
@@ -2571,7 +2592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>99</v>
       </c>
@@ -2603,7 +2624,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>99</v>
       </c>
@@ -2634,8 +2655,11 @@
       <c r="J40">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M40" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>99</v>
       </c>
@@ -2667,7 +2691,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>99</v>
       </c>
@@ -2699,7 +2723,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>99</v>
       </c>
@@ -2731,7 +2755,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>99</v>
       </c>
@@ -2766,7 +2790,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>99</v>
       </c>
@@ -2801,7 +2825,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>99</v>
       </c>
@@ -2833,7 +2857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>99</v>
       </c>
@@ -2865,7 +2889,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>99</v>
       </c>

</xml_diff>

<commit_message>
error in 2022/23 Q2 (c)
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmurphy/wit/archive/2025-26/modules/Discrete_Mathematics/exams/study_dashboard/Discrete_Mathematics_Exam_Viewer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58347C62-2D6A-AD4D-AF30-4BA4641B8487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91558143-3E59-E24F-A5DB-29FC1D5FE13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2640" windowWidth="30240" windowHeight="15100" xr2:uid="{422AB7C4-DC60-EF4B-B76F-C5BB3A29986B}"/>
+    <workbookView xWindow="0" yWindow="2640" windowWidth="30240" windowHeight="11320" xr2:uid="{422AB7C4-DC60-EF4B-B76F-C5BB3A29986B}"/>
   </bookViews>
   <sheets>
     <sheet name="questions_2" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="152">
   <si>
     <t>paper</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t>Error in solution - the calculation shown for (iii) is from an earlier version of the question.</t>
+  </si>
+  <si>
+    <t>Error in solution - solution should be 2/2^8  = 1/2^7, since they all could be wearing a red dress or all wearing a blue dress.</t>
   </si>
 </sst>
 </file>
@@ -1335,9 +1338,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C95249E-C714-E54A-906E-011FA13AE7C6}">
   <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="214" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="214" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2690,6 +2693,9 @@
       <c r="J41">
         <v>4</v>
       </c>
+      <c r="M41" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">

</xml_diff>